<commit_message>
Updated Leave Card 1/29/2024 4:47 pm
</commit_message>
<xml_diff>
--- a/CASUAL/LA DSWD-CCR/BELOSTRINO, JULIETA.xlsx
+++ b/CASUAL/LA DSWD-CCR/BELOSTRINO, JULIETA.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="107">
   <si>
     <t>PERIOD</t>
   </si>
@@ -355,6 +355,9 @@
   </si>
   <si>
     <t>UT(0-0-10)</t>
+  </si>
+  <si>
+    <t>2024</t>
   </si>
 </sst>
 </file>
@@ -1295,7 +1298,7 @@
         <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3B5D8F3C-4FD5-4318-83F6-163B56792B3A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B5D8F3C-4FD5-4318-83F6-163B56792B3A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1338,7 +1341,7 @@
         <xdr:cNvPr id="5" name="TextBox 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A0BAE224-67DC-A2F7-0A1F-28CB86DFB7CA}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0BAE224-67DC-A2F7-0A1F-28CB86DFB7CA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1402,7 +1405,7 @@
         <xdr:cNvPr id="4" name="Arrow: Left 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7243AC54-FD55-C7CF-DEF3-E45E6F99CAA1}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7243AC54-FD55-C7CF-DEF3-E45E6F99CAA1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1462,7 +1465,7 @@
         <xdr:cNvPr id="8" name="Oval 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6CEC4AD9-D5D6-0CFD-8D82-CC23F90E3707}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CEC4AD9-D5D6-0CFD-8D82-CC23F90E3707}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1528,7 +1531,7 @@
         <xdr:cNvPr id="9" name="Arrow: Left-Right 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EAE8B24D-B9B9-4AB0-AE94-782594B55A03}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAE8B24D-B9B9-4AB0-AE94-782594B55A03}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1591,7 +1594,7 @@
         <xdr:cNvPr id="10" name="TextBox 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D163C4F0-3D7F-3E52-4B17-0D29F1241915}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D163C4F0-3D7F-3E52-4B17-0D29F1241915}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1689,7 +1692,7 @@
         <xdr:cNvPr id="14" name="Straight Arrow Connector 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{642CA079-93A1-34E3-CEF5-F7D33015D895}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{642CA079-93A1-34E3-CEF5-F7D33015D895}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1748,7 +1751,7 @@
         <xdr:cNvPr id="19" name="TextBox 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{784FECEA-1780-3E7F-7EBB-9F8254797C91}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{784FECEA-1780-3E7F-7EBB-9F8254797C91}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1813,7 +1816,7 @@
         <xdr:cNvPr id="20" name="Picture 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5DCCE859-255F-F039-E92D-1510F02C6167}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DCCE859-255F-F039-E92D-1510F02C6167}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1856,7 +1859,7 @@
         <xdr:cNvPr id="21" name="TextBox 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0A7AA7C6-9540-EB37-E3D2-9A2A68BD6824}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A7AA7C6-9540-EB37-E3D2-9A2A68BD6824}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1931,7 +1934,7 @@
         <xdr:cNvPr id="22" name="TextBox 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F1674299-9801-A253-3871-18715F4FF740}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1674299-9801-A253-3871-18715F4FF740}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2117,7 +2120,7 @@
         <xdr:cNvPr id="23" name="Oval 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{66C92862-99CA-461F-932E-30DFD0874402}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66C92862-99CA-461F-932E-30DFD0874402}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2183,7 +2186,7 @@
         <xdr:cNvPr id="24" name="Straight Arrow Connector 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FD20A152-8288-4C69-BE76-AD8E41A960CE}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD20A152-8288-4C69-BE76-AD8E41A960CE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2241,7 +2244,7 @@
         <xdr:cNvPr id="26" name="Oval 25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EE7E56BE-0B3E-4110-A5A9-44C888A46B90}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE7E56BE-0B3E-4110-A5A9-44C888A46B90}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2307,7 +2310,7 @@
         <xdr:cNvPr id="27" name="Straight Arrow Connector 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C33E41C1-1592-4272-A561-4833666913C5}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C33E41C1-1592-4272-A561-4833666913C5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2363,7 +2366,7 @@
         <xdr:cNvPr id="30" name="TextBox 29">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6C655B57-0D66-4740-B73E-75D1E106F99A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C655B57-0D66-4740-B73E-75D1E106F99A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2438,7 +2441,7 @@
         <xdr:cNvPr id="31" name="Picture 30">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0284C105-1E11-4529-B509-D655B8C5279A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0284C105-1E11-4529-B509-D655B8C5279A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2481,7 +2484,7 @@
         <xdr:cNvPr id="32" name="Oval 31">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E73E9A40-2B3C-47DC-9C07-7C65795CE0A2}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E73E9A40-2B3C-47DC-9C07-7C65795CE0A2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2547,7 +2550,7 @@
         <xdr:cNvPr id="33" name="Straight Arrow Connector 32">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{32002197-8137-42BA-B3E7-2690738DB64B}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32002197-8137-42BA-B3E7-2690738DB64B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2603,7 +2606,7 @@
         <xdr:cNvPr id="34" name="TextBox 33">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A781E01A-37B6-4259-9759-556FE6893D51}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A781E01A-37B6-4259-9759-556FE6893D51}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2699,7 +2702,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A8:K142" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A8:K143" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
   <tableColumns count="11">
     <tableColumn id="1" name="PERIOD" dataDxfId="25"/>
     <tableColumn id="2" name="PARTICULARS" dataDxfId="24"/>
@@ -3076,12 +3079,12 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:K142"/>
+  <dimension ref="A2:M143"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3690" topLeftCell="A61" activePane="bottomLeft"/>
-      <selection activeCell="E9" sqref="E9"/>
-      <selection pane="bottomLeft" activeCell="F78" sqref="F78"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3690" topLeftCell="A85" activePane="bottomLeft"/>
+      <selection activeCell="M9" sqref="M9"/>
+      <selection pane="bottomLeft" activeCell="N92" sqref="N92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3099,7 +3102,7 @@
     <col min="11" max="11" width="24.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
         <v>9</v>
       </c>
@@ -3120,7 +3123,7 @@
       <c r="J2" s="54"/>
       <c r="K2" s="55"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>15</v>
       </c>
@@ -3138,7 +3141,7 @@
       <c r="J3" s="56"/>
       <c r="K3" s="57"/>
     </row>
-    <row r="4" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>16</v>
       </c>
@@ -3160,7 +3163,7 @@
       <c r="J4" s="54"/>
       <c r="K4" s="55"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
       <c r="H5" s="27" t="s">
         <v>18</v>
@@ -3168,7 +3171,7 @@
       <c r="I5" s="27"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="17"/>
       <c r="B6" s="8"/>
       <c r="C6" s="31"/>
@@ -3181,7 +3184,7 @@
       <c r="J6" s="8"/>
       <c r="K6" s="19"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
       <c r="C7" s="52" t="s">
@@ -3198,7 +3201,7 @@
       <c r="J7" s="52"/>
       <c r="K7" s="14"/>
     </row>
-    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>0</v>
       </c>
@@ -3233,7 +3236,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="23"/>
       <c r="B9" s="24" t="s">
         <v>23</v>
@@ -3242,7 +3245,7 @@
       <c r="D9" s="11"/>
       <c r="E9" s="13">
         <f>SUM(Table1[EARNED])-SUM(Table1[Absence Undertime W/ Pay])</f>
-        <v>33.996999999999993</v>
+        <v>35.246999999999993</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="13" t="str">
@@ -3252,12 +3255,13 @@
       <c r="H9" s="11"/>
       <c r="I9" s="13">
         <f>SUM(Table1[[EARNED ]])-SUM(Table1[Absence Undertime  W/ Pay])</f>
-        <v>58.75</v>
+        <v>65</v>
       </c>
       <c r="J9" s="11"/>
       <c r="K9" s="20"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M9" s="46"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="48" t="s">
         <v>45</v>
       </c>
@@ -3279,7 +3283,7 @@
       <c r="J10" s="11"/>
       <c r="K10" s="20"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="40">
         <v>43101</v>
       </c>
@@ -3299,7 +3303,7 @@
       <c r="J11" s="11"/>
       <c r="K11" s="20"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="40">
         <v>43132</v>
       </c>
@@ -3319,7 +3323,7 @@
       <c r="J12" s="11"/>
       <c r="K12" s="20"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="40">
         <v>43160</v>
       </c>
@@ -3339,7 +3343,7 @@
       <c r="J13" s="11"/>
       <c r="K13" s="20"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="40">
         <v>43191</v>
       </c>
@@ -3359,7 +3363,7 @@
       <c r="J14" s="11"/>
       <c r="K14" s="20"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="40">
         <v>43221</v>
       </c>
@@ -3379,7 +3383,7 @@
       <c r="J15" s="11"/>
       <c r="K15" s="20"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="40">
         <v>43252</v>
       </c>
@@ -5136,15 +5140,19 @@
       <c r="K98" s="20"/>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A99" s="40"/>
+      <c r="A99" s="40">
+        <v>45139</v>
+      </c>
       <c r="B99" s="20"/>
-      <c r="C99" s="13"/>
+      <c r="C99" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D99" s="39"/>
       <c r="E99" s="9"/>
       <c r="F99" s="20"/>
-      <c r="G99" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G99" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H99" s="39"/>
       <c r="I99" s="9"/>
@@ -5152,15 +5160,19 @@
       <c r="K99" s="20"/>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A100" s="40"/>
+      <c r="A100" s="40">
+        <v>45170</v>
+      </c>
       <c r="B100" s="20"/>
-      <c r="C100" s="13"/>
+      <c r="C100" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D100" s="39"/>
       <c r="E100" s="9"/>
       <c r="F100" s="20"/>
-      <c r="G100" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G100" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H100" s="39"/>
       <c r="I100" s="9"/>
@@ -5168,15 +5180,19 @@
       <c r="K100" s="20"/>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A101" s="40"/>
+      <c r="A101" s="40">
+        <v>45200</v>
+      </c>
       <c r="B101" s="20"/>
-      <c r="C101" s="13"/>
+      <c r="C101" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D101" s="39"/>
       <c r="E101" s="9"/>
       <c r="F101" s="20"/>
-      <c r="G101" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G101" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H101" s="39"/>
       <c r="I101" s="9"/>
@@ -5184,15 +5200,19 @@
       <c r="K101" s="20"/>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A102" s="40"/>
+      <c r="A102" s="40">
+        <v>45231</v>
+      </c>
       <c r="B102" s="20"/>
-      <c r="C102" s="13"/>
+      <c r="C102" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D102" s="39"/>
       <c r="E102" s="9"/>
       <c r="F102" s="20"/>
-      <c r="G102" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G102" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H102" s="39"/>
       <c r="I102" s="9"/>
@@ -5200,15 +5220,23 @@
       <c r="K102" s="20"/>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A103" s="40"/>
-      <c r="B103" s="20"/>
-      <c r="C103" s="13"/>
-      <c r="D103" s="39"/>
+      <c r="A103" s="40">
+        <v>45261</v>
+      </c>
+      <c r="B103" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C103" s="13">
+        <v>1.25</v>
+      </c>
+      <c r="D103" s="39">
+        <v>5</v>
+      </c>
       <c r="E103" s="9"/>
       <c r="F103" s="20"/>
-      <c r="G103" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G103" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H103" s="39"/>
       <c r="I103" s="9"/>
@@ -5216,7 +5244,9 @@
       <c r="K103" s="20"/>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A104" s="40"/>
+      <c r="A104" s="48" t="s">
+        <v>106</v>
+      </c>
       <c r="B104" s="20"/>
       <c r="C104" s="13"/>
       <c r="D104" s="39"/>
@@ -5232,7 +5262,9 @@
       <c r="K104" s="20"/>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A105" s="40"/>
+      <c r="A105" s="40">
+        <v>45292</v>
+      </c>
       <c r="B105" s="20"/>
       <c r="C105" s="13"/>
       <c r="D105" s="39"/>
@@ -5248,7 +5280,9 @@
       <c r="K105" s="20"/>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A106" s="40"/>
+      <c r="A106" s="40">
+        <v>45323</v>
+      </c>
       <c r="B106" s="20"/>
       <c r="C106" s="13"/>
       <c r="D106" s="39"/>
@@ -5264,7 +5298,9 @@
       <c r="K106" s="20"/>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A107" s="40"/>
+      <c r="A107" s="40">
+        <v>45352</v>
+      </c>
       <c r="B107" s="20"/>
       <c r="C107" s="13"/>
       <c r="D107" s="39"/>
@@ -5824,20 +5860,36 @@
       <c r="K141" s="20"/>
     </row>
     <row r="142" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A142" s="41"/>
-      <c r="B142" s="15"/>
-      <c r="C142" s="42"/>
-      <c r="D142" s="43"/>
+      <c r="A142" s="40"/>
+      <c r="B142" s="20"/>
+      <c r="C142" s="13"/>
+      <c r="D142" s="39"/>
       <c r="E142" s="9"/>
-      <c r="F142" s="15"/>
+      <c r="F142" s="20"/>
       <c r="G142" s="13" t="str">
         <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
         <v/>
       </c>
-      <c r="H142" s="43"/>
+      <c r="H142" s="39"/>
       <c r="I142" s="9"/>
-      <c r="J142" s="12"/>
-      <c r="K142" s="15"/>
+      <c r="J142" s="11"/>
+      <c r="K142" s="20"/>
+    </row>
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A143" s="41"/>
+      <c r="B143" s="15"/>
+      <c r="C143" s="42"/>
+      <c r="D143" s="43"/>
+      <c r="E143" s="9"/>
+      <c r="F143" s="15"/>
+      <c r="G143" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H143" s="43"/>
+      <c r="I143" s="9"/>
+      <c r="J143" s="12"/>
+      <c r="K143" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -7445,17 +7497,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="G7:J7"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="J3:K3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="G7:J7"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4">

</xml_diff>